<commit_message>
Just changed the name of the sheet.
</commit_message>
<xml_diff>
--- a/Circuits/Voltage distribution/Different voltage levels summary.xlsx
+++ b/Circuits/Voltage distribution/Different voltage levels summary.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentmdh-my.sharepoint.com/personal/fnl18001_student_mdu_se/Documents/Robotics_program_university/Ongoing_courses/DVA490/SSL-Hardware-Development/Circuits/Voltage distribution/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fnl18001\OneDrive - Mälardalens universitet\Robotics_program_university\Ongoing_courses\DVA490\SSL-Hardware-Development\Circuits\Voltage distribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{F987802B-0752-49A9-A4EA-86FDF67BEAB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{C0043B36-B7FF-4090-9189-6BCB265B9024}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{F987802B-0752-49A9-A4EA-86FDF67BEAB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{3DE6E4CF-48C0-470A-A3D8-AD3E182258C5}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" xr2:uid="{85820359-25C7-4DA9-A692-6E4FD3191B26}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Different Voltage Levels" sheetId="1" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
@@ -492,7 +492,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,6 +607,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d249f748-2859-45fd-a747-2e289ca8c4c8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009886D6671A81FB4788FD8CEEA40A8F5A" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="58e97b55baf7639b4d456708924fe61d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d249f748-2859-45fd-a747-2e289ca8c4c8" xmlns:ns4="52418e62-0214-4ef5-8ea7-4e8018f8a97c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="209907aae15c3e25da3474742949ee53" ns3:_="" ns4:_="">
     <xsd:import namespace="d249f748-2859-45fd-a747-2e289ca8c4c8"/>
@@ -839,24 +856,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d249f748-2859-45fd-a747-2e289ca8c4c8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E9CE8B-4C7A-4652-940C-AA90DD44DBCB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="52418e62-0214-4ef5-8ea7-4e8018f8a97c"/>
+    <ds:schemaRef ds:uri="d249f748-2859-45fd-a747-2e289ca8c4c8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77ACBEFC-D395-432F-9508-6676C0FF599E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62452C2F-6131-4516-8238-F0DF6602DE87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -873,29 +898,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77ACBEFC-D395-432F-9508-6676C0FF599E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E9CE8B-4C7A-4652-940C-AA90DD44DBCB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="d249f748-2859-45fd-a747-2e289ca8c4c8"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="52418e62-0214-4ef5-8ea7-4e8018f8a97c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>